<commit_message>
Umbau auf Einzel-Sheets, Default-Field im Dialog nun einstellbar
</commit_message>
<xml_diff>
--- a/Iteration 2try2/Mitarbeiterzeiten/KL/MA_KL.xlsx
+++ b/Iteration 2try2/Mitarbeiterzeiten/KL/MA_KL.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UBXGitHub\HtmXRechnung\Iteration 2try2\Mitarbeiterzeiten\KL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC97174C-3E3F-4629-B841-1FEFAEFBC272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35513E76-A0E3-4CE5-AC05-BE733E58DC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="675" windowWidth="33570" windowHeight="20235" tabRatio="373" firstSheet="2" activeTab="2" xr2:uid="{5A353484-0E68-4912-BD2B-362C94CA2B03}"/>
+    <workbookView xWindow="930" yWindow="1155" windowWidth="33570" windowHeight="20235" tabRatio="373" firstSheet="1" activeTab="1" xr2:uid="{5A353484-0E68-4912-BD2B-362C94CA2B03}"/>
   </bookViews>
   <sheets>
-    <sheet name="Settings" sheetId="30" state="veryHidden" r:id="rId1"/>
-    <sheet name="Makros" sheetId="29" state="veryHidden" r:id="rId2"/>
-    <sheet name="MA KL" sheetId="27" r:id="rId3"/>
+    <sheet name="Makros" sheetId="29" state="veryHidden" r:id="rId1"/>
+    <sheet name="MA KL" sheetId="27" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="153">
   <si>
     <t>Datum</t>
   </si>
@@ -485,49 +484,18 @@
     <t>89EBA500-2E9B-43BA-88AF-7B1DA3B998E2</t>
   </si>
   <si>
-    <t>Std.-satz</t>
-  </si>
-  <si>
-    <t>MA HA</t>
-  </si>
-  <si>
-    <t>MA KL</t>
-  </si>
-  <si>
-    <t>MA ZD</t>
-  </si>
-  <si>
-    <t>MA-Kürzel</t>
-  </si>
-  <si>
-    <t>Kanzlei-Zeiterfassung - Grundeinstellungen</t>
-  </si>
-  <si>
-    <t>Passwort:</t>
-  </si>
-  <si>
-    <t>BierBaum67</t>
-  </si>
-  <si>
     <t>M</t>
-  </si>
-  <si>
-    <t>Suchpfad für Zeiterfassungsdateien:</t>
-  </si>
-  <si>
-    <t>.\Mitarbeiterzeiten\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€]_-;\-* #,##0.00\ [$€]_-;_-* \-??\ [$€]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.00&quot; €&quot;"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -555,25 +523,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -622,7 +571,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -666,9 +615,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Ergebnis 1" xfId="1" xr:uid="{169007C4-7436-4EB5-9583-724C779FE769}"/>
@@ -688,230 +634,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>2152650</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Button 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
-                </a:rPr>
-                <a:t>Zeige erweiterte Einstellungen und erlaube Einstellungsänderungen</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>1047750</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1026" name="Button 2" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1026"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
-                </a:rPr>
-                <a:t>Spaltenschutz starten</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>47625</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>2162175</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="Button 3" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1027"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="de-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
-                </a:rPr>
-                <a:t>Einstellungen schließen</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1261,154 +983,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A3C084-4CD3-4EE4-8348-2D2B219E4AE0}">
-  <sheetPr codeName="Tabelle4"/>
-  <dimension ref="A1:G11"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="B3" t="s">
-        <v>162</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="G3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F8" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F9" t="s">
-        <v>153</v>
-      </c>
-      <c r="G9" s="17">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F10" t="s">
-        <v>154</v>
-      </c>
-      <c r="G10" s="17">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G11" s="17">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="xh7aDVyVHGpn8jCjM/7Jv7ER/BhMb53k3Wia87tVHusQURDwEh+nnG5GW3/acQ2NxaH0qX1XzbVLtg8Xw9r2WA==" saltValue="ThkM5Et/dc8Ugtgz65oTRQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId4" name="Button 1">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!SettingsSpaltenschutzAufheben">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>57150</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>2152650</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId5" name="Button 2">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!SettingsSpaltenSchutzStarten">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>1047750</xdr:colOff>
-                    <xdr:row>5</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1027" r:id="rId6" name="Button 3">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!HideAllSettingItems">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>47625</xdr:colOff>
-                    <xdr:row>18</xdr:row>
-                    <xdr:rowOff>85725</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>2162175</xdr:colOff>
-                    <xdr:row>21</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F252DCB4-EA17-43BC-9D22-3E5D760FACB1}">
   <sheetPr codeName="AlleMakros"/>
   <dimension ref="A1"/>
@@ -1421,14 +995,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{024D5387-D9FF-4707-BB1F-73F4260D4163}">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2672,7 +2246,7 @@
         <v>60263</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D61" t="s">
         <v>6</v>
@@ -3177,20 +2751,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=customUI/customUI14.xml><?xml version="1.0" encoding="utf-8"?>
-<customUI xmlns="http://schemas.microsoft.com/office/2006/01/customui">
-  <ribbon>
-    <tabs>
-      <tab id="StBAhting" label="StB Ahting">
-        <group id="StBAhtinGroup" label="StB Ahting-Menü">
-          <button id="StBAbrechnung" label="Abrechnung Zeiten" imageMso="DateAndTimeInsert" onAction="Dialogfunktionen.StartAbrechnung"/>
-          <button id="Settings" label="Zeige Einstellungsseite" imageMso="OmsCustomizeLayout" onAction="Dialogfunktionen.ShowSettings"/>
-          <button id="Abgleich" label="Erstelle Abgleichliste für Dublettensuche" imageMso="ReviewCompareTwoVersions" onAction="Abgleich.ErzeugeAbgleichSheet"/>
-        </group>
-      </tab>
-    </tabs>
-  </ribbon>
-</customUI>
 </file>
</xml_diff>

<commit_message>
WIP: Einbau Listbox-namen sammeln
</commit_message>
<xml_diff>
--- a/Iteration 2try2/Mitarbeiterzeiten/KL/MA_KL.xlsx
+++ b/Iteration 2try2/Mitarbeiterzeiten/KL/MA_KL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UBXGitHub\HtmXRechnung\Iteration 2try2\Mitarbeiterzeiten\KL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35513E76-A0E3-4CE5-AC05-BE733E58DC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13FE72C-E494-4663-BC61-CE5F9CDD9C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="1155" windowWidth="33570" windowHeight="20235" tabRatio="373" firstSheet="1" activeTab="1" xr2:uid="{5A353484-0E68-4912-BD2B-362C94CA2B03}"/>
+    <workbookView xWindow="3135" yWindow="60" windowWidth="35265" windowHeight="21870" tabRatio="373" firstSheet="1" activeTab="1" xr2:uid="{5A353484-0E68-4912-BD2B-362C94CA2B03}"/>
   </bookViews>
   <sheets>
     <sheet name="Makros" sheetId="29" state="veryHidden" r:id="rId1"/>

</xml_diff>